<commit_message>
sample download cap table file
</commit_message>
<xml_diff>
--- a/public/28912SAIAS232/investor-cap-table-upload.xlsx
+++ b/public/28912SAIAS232/investor-cap-table-upload.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>Property or Fund Name</t>
   </si>
@@ -19,10 +19,16 @@
     <t>Company Name</t>
   </si>
   <si>
-    <t>Palms DST</t>
-  </si>
-  <si>
-    <t>Sample Test Group LLC</t>
+    <t>Company Tax ID #</t>
+  </si>
+  <si>
+    <t>Company Debit Account</t>
+  </si>
+  <si>
+    <t>Sample Fund / Property Name</t>
+  </si>
+  <si>
+    <t>Sample Company</t>
   </si>
   <si>
     <t>Investor Name on Bank Account</t>
@@ -38,6 +44,15 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>ACH ABA Routing Number</t>
+  </si>
+  <si>
+    <t>Bank Account Number</t>
+  </si>
+  <si>
+    <t>Account Type</t>
   </si>
   <si>
     <t>Sample Name 1 Partners</t>
@@ -54,6 +69,12 @@
     </r>
   </si>
   <si>
+    <t>0028483226</t>
+  </si>
+  <si>
+    <t>Checking</t>
+  </si>
+  <si>
     <t>Sample Name 2 Partners</t>
   </si>
   <si>
@@ -65,6 +86,20 @@
         <rFont val="Calibri"/>
       </rPr>
       <t>sample2@email.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Sample Name 3 Partners</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>sample3@email.com</t>
     </r>
   </si>
   <si>
@@ -157,7 +192,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -167,16 +202,31 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -185,10 +235,19 @@
     <xf numFmtId="14" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -217,7 +276,7 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ff0563c1"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -416,17 +475,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -454,10 +513,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -705,12 +764,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -997,7 +1056,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1025,10 +1084,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1279,7 +1338,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1288,9 +1347,12 @@
     <col min="1" max="1" width="27.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.8516" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1719" style="1" customWidth="1"/>
     <col min="5" max="5" width="27.6719" style="1" customWidth="1"/>
-    <col min="6" max="256" width="10.8516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.8516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="1" customWidth="1"/>
+    <col min="9" max="256" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
@@ -1300,113 +1362,186 @@
       <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" t="s" s="5">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s" s="6">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7">
+        <v>9114119079</v>
+      </c>
+      <c r="D2" s="8">
+        <v>4870149079</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" ht="17" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" ht="17" customHeight="1">
-      <c r="A4" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s" s="5">
+      <c r="A4" t="s" s="10">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="5">
+      <c r="B4" t="s" s="10">
         <v>7</v>
       </c>
-      <c r="E4" t="s" s="5">
+      <c r="C4" t="s" s="10">
         <v>8</v>
+      </c>
+      <c r="D4" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s" s="11">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s" s="11">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s" s="11">
+        <v>13</v>
       </c>
     </row>
     <row r="5" ht="17" customHeight="1">
-      <c r="A5" t="s" s="6">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7">
-        <f>60%</f>
-        <v>0.6</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="A5" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="B5" s="12">
+        <f>D5/$D$9</f>
+        <v>0.595238095238095</v>
+      </c>
+      <c r="C5" s="13">
         <v>43555</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="14">
         <v>12500000</v>
       </c>
-      <c r="E5" t="s" s="4">
-        <v>10</v>
+      <c r="E5" t="s" s="15">
+        <v>15</v>
+      </c>
+      <c r="F5" s="8">
+        <v>125000105</v>
+      </c>
+      <c r="G5" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s" s="17">
+        <v>17</v>
       </c>
     </row>
     <row r="6" ht="17" customHeight="1">
-      <c r="A6" t="s" s="6">
-        <v>11</v>
-      </c>
-      <c r="B6" s="7">
-        <f>40%</f>
-        <v>0.4</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="A6" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="B6" s="12">
+        <f>D6/$D$9</f>
+        <v>0.261904761904762</v>
+      </c>
+      <c r="C6" s="13">
         <v>43555</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="14">
         <v>5500000</v>
       </c>
-      <c r="E6" t="s" s="4">
-        <v>12</v>
+      <c r="E6" t="s" s="15">
+        <v>19</v>
+      </c>
+      <c r="F6" s="8">
+        <v>314074269</v>
+      </c>
+      <c r="G6" s="8">
+        <v>8406728894</v>
+      </c>
+      <c r="H6" t="s" s="17">
+        <v>17</v>
       </c>
     </row>
     <row r="7" ht="17" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="4"/>
+      <c r="A7" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B7" s="12">
+        <f>D7/$D$9</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="C7" s="13">
+        <v>43555</v>
+      </c>
+      <c r="D7" s="14">
+        <v>3000000</v>
+      </c>
+      <c r="E7" t="s" s="15">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8">
+        <v>121100782</v>
+      </c>
+      <c r="G7" s="8">
+        <v>93728372318</v>
+      </c>
+      <c r="H7" t="s" s="17">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" ht="17" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" ht="17" customHeight="1">
-      <c r="A9" t="s" s="4">
-        <v>13</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="10">
+      <c r="A9" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="18">
         <f>SUM(D5:D8)</f>
-        <v>18000000</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>21000000</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" ht="17" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:D7 D9">
@@ -1417,6 +1552,7 @@
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" location="" tooltip="" display="sample1@email.com"/>
     <hyperlink ref="E6" r:id="rId2" location="" tooltip="" display="sample2@email.com"/>
+    <hyperlink ref="E7" r:id="rId3" location="" tooltip="" display="sample3@email.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>